<commit_message>
task3 and task4 - re-run after loss function change
</commit_message>
<xml_diff>
--- a/Assignment3/output/task4 output.xlsx
+++ b/Assignment3/output/task4 output.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgazit\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC1E7ABF-7705-4B3D-BC76-72E97FB7F8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1C4A417-0456-402A-AAFF-CB64F99FEED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="task4" sheetId="1" r:id="rId1"/>
+    <sheet name="task4 output" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">task4!$A$1:$D$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'task4 output'!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -883,7 +883,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +919,7 @@
         <v>0.01</v>
       </c>
       <c r="D2">
-        <v>3.2099999999999997E-2</v>
+        <v>0.10390000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>1E-3</v>
       </c>
       <c r="D3">
-        <v>3.2899999999999999E-2</v>
+        <v>0.10929999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -947,7 +947,7 @@
         <v>1E-4</v>
       </c>
       <c r="D4">
-        <v>8.0399999999999999E-2</v>
+        <v>0.28899999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>0.01</v>
       </c>
       <c r="D5">
-        <v>2.9700000000000001E-2</v>
+        <v>0.1099</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>1E-3</v>
       </c>
       <c r="D6">
-        <v>6.6000000000000003E-2</v>
+        <v>0.22900000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>1E-4</v>
       </c>
       <c r="D7">
-        <v>0.1389</v>
+        <v>0.8266</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
         <v>0.01</v>
       </c>
       <c r="D8">
-        <v>2.7900000000000001E-2</v>
+        <v>0.1174</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>1E-3</v>
       </c>
       <c r="D9">
-        <v>2.29E-2</v>
+        <v>7.3899999999999993E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1031,21 +1031,21 @@
         <v>1E-4</v>
       </c>
       <c r="D10">
-        <v>6.08E-2</v>
+        <v>0.20880000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>500</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>1000</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>0.01</v>
       </c>
       <c r="D11" s="3">
-        <v>2.2200000000000001E-2</v>
+        <v>6.8599999999999994E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1059,7 @@
         <v>1E-3</v>
       </c>
       <c r="D12">
-        <v>4.6600000000000003E-2</v>
+        <v>0.1555</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,12 +1073,11 @@
         <v>1E-4</v>
       </c>
       <c r="D13">
-        <v>0.1032</v>
+        <v>0.4456</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>